<commit_message>
removed unused global variables
</commit_message>
<xml_diff>
--- a/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.0.xlsx
+++ b/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.0.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="menu_urls" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="submenu_urls" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="item_info" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -630,135 +628,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>menu</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>item</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quantity</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Date Crown Lulu Dates</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>400 gm</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>৳ 249</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">*Features an elongated oval *shape and smooth, glossy skin *Rich in fibers *High in potassium *Low in sodium *Source of magnesium *Naturally sweet flavour makes these dates a perfect choice for adding to cakes, cookies, and more *Ideal on-the-go snacking option *Can be stored in an airtight container to preserve freshness *Vegan *Gluten Free *No added sugar and preservatives </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Popular</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ajwa Premium Dates</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>500 gm</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>৳ 693</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Origin: Saudi Arabia Dry,Semi-Moist,Oragnic,Dairy Free,Nut Free,Egg Free Ajwa dates Ingredients: Mabroom/Morium Dates/ Khejur Imported Dates. Halal Net Weight: 500gm Ajwa Dates (0.25 cup) contains 30g total carbs, 27g net carbs, 0g fat, 1g protein, and 120 calories</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Popular</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
done with functional code
</commit_message>
<xml_diff>
--- a/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.0.xlsx
+++ b/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.0.xlsx
@@ -1895,20 +1895,24 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Crown Dabbas Dates</t>
+          <t>Date Crown Lulu Dates</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1 kg</t>
+          <t>400 gm</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>৳ 549</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>৳ 249</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*Features an elongated oval *shape and smooth, glossy skin *Rich in fibers *High in potassium *Low in sodium *Source of magnesium *Naturally sweet flavour makes these dates a perfect choice for adding to cakes, cookies, and more *Ideal on-the-go snacking option *Can be stored in an airtight container to preserve freshness *Vegan *Gluten Free *No added sugar and preservatives </t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>Popular</t>
@@ -1918,16 +1922,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chaldal Sippy Orange Drinks 500 gm And Crown Dabbas Dates 1 kg (Combo Offer)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>Maryam Premium Dates</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>500 gm</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>৳ 769</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>৳ 599</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Dry,Semi-Moist,Oragnic,Dairy Free,Nut Free,Egg Ingredients: Mabroom/Morium Dates/ Khejur Imported Dates. Halal Net Weight: 500gm</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Popular</t>
@@ -1937,22 +1949,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Deshi Peyaj (Local Onion) ± 50 gm</t>
+          <t>Chaldal Premium Rui Fish Headless Curry Cut and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1 kg</t>
+          <t>500 gm</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>৳ 69</t>
+          <t>৳ 369</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>30-35 pcs  Though all vegetables are important for health, certain kinds offer unique benefits.  Onions are members of the Allium genus of flowering plants that also includes garlic, shallots, leeks and chives.  These vegetables contain various vitamins, minerals and potent plant compounds that have been shown to promote health in many ways.  In fact, the medicinal properties of onions have been recognized since ancient times, when they were used to treat ailments like headaches, heart disease and mouth sores.  Nutritional facts/Ingredients : Benefits: -Packed With Nutrients -May Benefit Heart Health -Loaded With Antioxidants -Contain Cancer-Fighting Compounds -Help Control Blood Sugar -May Boost Bone Density -Have Antibacterial Properties -May Boost Digestive Health -Easy to Add to Your Diet.</t>
+          <t>Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Rui Fish Headless Curry Cut (7-11 pcs) ±30 gm 500 gm  We are offering Premium Rui With means This fishes are 100% dish bread and specially collected from Rajshahi.  Our RUI fish are mentioned as Medium size with means each of the live fish will have to be between 1.8 KG to 2.5 KG.  Bengali cut pieces of Freshwater Rui that's caught fresh, cut, cleaned.  These are Medium pieces of Bengali Cuts of freshwater Rui, that are perfect for curries or fish fry. Rui is a soft-textured bony fish with a subtle flavour.  Chaldal fish &amp; seafood is sourced from approved local fishermen Regularly, they contain no added chemicals.  Features of our premium Rui fish:  1. 100% native cotton fish. 2. Our fishes are sourced from selected fish farms in Rajshahi where systematic fish farming is ensured. 3. Our premium fish are processed under our own supervision by skilled artisans. 4. Clean water is used when poaching premium fish. 5. Safe packing is done in compliance with complete hygiene rules. 6. Fish are caught and processed on the same day.  45-50 Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1964,22 +1976,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Potato Regular (± 50 gm)</t>
+          <t>Chaldal Premium Koi Fish Medium and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1 kg</t>
+          <t>500 gm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>৳ 45</t>
+          <t>৳ 269</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">18 -22 pcs  Buy regular potato from us which provides you with dietary fiber, potassium, vitamins, etc. Regular potato provides 9-10 percent of your daily need. Regular potatoes offer more of this nutrient which helps control your blood pressure. Make a good curry with regular potato. You can make French fries and you can enjoy with your family members. </t>
+          <t xml:space="preserve">Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Koi Fish Medium (7-9 pcs) ±30 gm 500 gm  Koi are freshwater fish that belong to the family of carp fish. Koi has a single centre bone and multiple small bones, that can be removed after cooking. It has firm skin and texture and an oily flavor. This cut consists of medium-sized, whole, cleaned &amp; gutted koi fish, with head, for your convenience. Koi fish can be enjoyed steamed, grilled, fried or in curries. They are widely enjoyed in Bengali cuisine, Tel Koi being a popular dish.  45-50  Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body. </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2024,7 +2036,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>৳ 35</t>
+          <t>৳ 29</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2041,20 +2053,24 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Crown Dabbas Dates</t>
+          <t>Date Crown Lulu Dates</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1 kg</t>
+          <t>400 gm</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>৳ 549</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>৳ 249</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*Features an elongated oval *shape and smooth, glossy skin *Rich in fibers *High in potassium *Low in sodium *Source of magnesium *Naturally sweet flavour makes these dates a perfect choice for adding to cakes, cookies, and more *Ideal on-the-go snacking option *Can be stored in an airtight container to preserve freshness *Vegan *Gluten Free *No added sugar and preservatives </t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>Dates (Khejur)</t>
@@ -2064,16 +2080,24 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chaldal Sippy Orange Drinks 500 gm And Crown Dabbas Dates 1 kg (Combo Offer)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>Maryam Premium Dates</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>500 gm</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>৳ 769</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>৳ 599</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Dry,Semi-Moist,Oragnic,Dairy Free,Nut Free,Egg Ingredients: Mabroom/Morium Dates/ Khejur Imported Dates. Halal Net Weight: 500gm</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>Dates (Khejur)</t>
@@ -2137,7 +2161,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chaldal Premium Pangas Fish Headless ±30 gm</t>
+          <t>Chaldal Premium Rui Fish Headless Curry Cut and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2147,12 +2171,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>৳ 199</t>
+          <t>৳ 369</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Pangas is a less bony fish, it has pink flesh and a mild smell which makes it popular. Pangas flesh is tender and has a moist &amp; sweet flavor. When cooked the flesh turns white and flaky.  Chaldal Pangas Curry Cut each pack contains 500gm which has 7 to 11 pics fish steak.  Pangas is a versatile fish that can be cooked in a variety of ways, including baking, grilling, frying, and steaming. It is a low-fat, low-calorie protein source that is rich in essential nutrients like Omega-3 fatty acids, vitamins B12 and D, and minerals such as phosphorus and selenium. Whether you are a professional chef or a home cook, Pangas fish is a great option for those who want to include more seafood in their diet. Order Pangas fish today and add a healthy, delicious, and easy-to-cook option to your menu!</t>
+          <t>Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Rui Fish Headless Curry Cut (7-11 pcs) ±30 gm 500 gm  We are offering Premium Rui With means This fishes are 100% dish bread and specially collected from Rajshahi.  Our RUI fish are mentioned as Medium size with means each of the live fish will have to be between 1.8 KG to 2.5 KG.  Bengali cut pieces of Freshwater Rui that's caught fresh, cut, cleaned.  These are Medium pieces of Bengali Cuts of freshwater Rui, that are perfect for curries or fish fry. Rui is a soft-textured bony fish with a subtle flavour.  Chaldal fish &amp; seafood is sourced from approved local fishermen Regularly, they contain no added chemicals.  Features of our premium Rui fish:  1. 100% native cotton fish. 2. Our fishes are sourced from selected fish farms in Rajshahi where systematic fish farming is ensured. 3. Our premium fish are processed under our own supervision by skilled artisans. 4. Clean water is used when poaching premium fish. 5. Safe packing is done in compliance with complete hygiene rules. 6. Fish are caught and processed on the same day.  45-50 Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2164,7 +2188,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chaldal Premium Koi Fish Medium (7-9 pcs) ±30 gm</t>
+          <t>Chaldal Premium Koi Fish Medium and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2174,12 +2198,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>৳ 239</t>
+          <t>৳ 269</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Koi are freshwater fish that belong to the family of carp fish. Koi has a single centre bone and multiple small bones, that can be removed after cooking. It has firm skin and texture and an oily flavor. This cut consists of medium-sized, whole, cleaned &amp; gutted koi fish, with head, for your convenience. Koi fish can be enjoyed steamed, grilled, fried or in curries. They are widely enjoyed in Bengali cuisine, Tel Koi being a popular dish.</t>
+          <t xml:space="preserve">Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Koi Fish Medium (7-9 pcs) ±30 gm 500 gm  Koi are freshwater fish that belong to the family of carp fish. Koi has a single centre bone and multiple small bones, that can be removed after cooking. It has firm skin and texture and an oily flavor. This cut consists of medium-sized, whole, cleaned &amp; gutted koi fish, with head, for your convenience. Koi fish can be enjoyed steamed, grilled, fried or in curries. They are widely enjoyed in Bengali cuisine, Tel Koi being a popular dish.  45-50  Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body. </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2191,22 +2215,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Horina Chingri (Shrimp) 60-70 pcs ±15 gm</t>
+          <t>Chaldal Premium Rui Fish Headless Curry Cut and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>250 gm</t>
+          <t>500 gm</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>৳ 229</t>
+          <t>৳ 369</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Before Processing this product live weight was 270 gm and the product quantity around 60-70 pcs.  Source: CULTURED /GHER  Horina Chingri Shiny, moist, and even slippery skin.In Khulna &amp; Shatkhira area best quality Horina Chingri is available. </t>
+          <t>Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Rui Fish Headless Curry Cut (7-11 pcs) ±30 gm 500 gm  We are offering Premium Rui With means This fishes are 100% dish bread and specially collected from Rajshahi.  Our RUI fish are mentioned as Medium size with means each of the live fish will have to be between 1.8 KG to 2.5 KG.  Bengali cut pieces of Freshwater Rui that's caught fresh, cut, cleaned.  These are Medium pieces of Bengali Cuts of freshwater Rui, that are perfect for curries or fish fry. Rui is a soft-textured bony fish with a subtle flavour.  Chaldal fish &amp; seafood is sourced from approved local fishermen Regularly, they contain no added chemicals.  Features of our premium Rui fish:  1. 100% native cotton fish. 2. Our fishes are sourced from selected fish farms in Rajshahi where systematic fish farming is ensured. 3. Our premium fish are processed under our own supervision by skilled artisans. 4. Clean water is used when poaching premium fish. 5. Safe packing is done in compliance with complete hygiene rules. 6. Fish are caught and processed on the same day.  45-50 Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2218,7 +2242,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bagda Chingri (Shrimp) 35-40 pcs ±30 gm</t>
+          <t>Chaldal Premium Koi Fish Medium and Deshi Roshun (Combo)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2228,12 +2252,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>৳ 469</t>
+          <t>৳ 269</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Before Processing this product live weight was 520 gm and the product quantity around 35-40 pcs.  Source:CULTURED /GHER  English Name: Tiger Prawn. Bengali Name: Bagda Chingri.Tiger prawns are large-bodied . Tiger prawns get their common name from the stripes that cover their shell..In Khulna &amp; Satkhira area best quality Tiger Prawn fish available. </t>
+          <t xml:space="preserve">Deshi Roshun (Garlic Local) ±25 gm 500 gm  Chaldal Premium Koi Fish Medium (7-9 pcs) ±30 gm 500 gm  Koi are freshwater fish that belong to the family of carp fish. Koi has a single centre bone and multiple small bones, that can be removed after cooking. It has firm skin and texture and an oily flavor. This cut consists of medium-sized, whole, cleaned &amp; gutted koi fish, with head, for your convenience. Koi fish can be enjoyed steamed, grilled, fried or in curries. They are widely enjoyed in Bengali cuisine, Tel Koi being a popular dish.  45-50  Garlic is an excellent source of minerals and vitamins that are essential for optimum health. The bulbs are one of the richest sources of potassium, iron, calcium, magnesium, manganese, zinc, and selenium. Selenium is a heart-healthy mineral, and is an important cofactor for antioxidant enzymes within the body. </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2245,24 +2269,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Broiler Chicken Skin On ± 50 gm</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>1 kg</t>
-        </is>
-      </c>
+          <t>Fresh Haleem Mix 200 gm And Halim Meat (Beef) ± 20 gm 300 gm (Combo Offer)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>৳ 329</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Before processing this product's live weight was 1.5-1.55 kg.  Broiler chickens are raised primarily for meat rather than to lay eggs. These poultry are often white and are bred to be large and very healthy, often with more breast meat for the consumer market. Broiler chicken breeds grow very fast and offer good value in terms of protein and calories.</t>
-        </is>
-      </c>
+          <t>৳ 259</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>Meat</t>
@@ -2272,22 +2288,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cock Chicken Skin Off ± 25 gm</t>
+          <t>Broiler Chicken Skin On ± 50 gm</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>500 gm</t>
+          <t>1 kg</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>৳ 299</t>
+          <t>৳ 329</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Before processing this product's live weight was 900-950 gm.  After Processed Weight: 500-550 gm. A cock is a sexually mature chicken over one year of age, also known as a rooster. Bonus definitions: A cockerel is a young male chicken that is not yet one year old. A pullet is a young female chicken that is fully feathered, is less than one year of age, and has not yet laid an egg. </t>
+          <t>Before processing this product's live weight was 1.5-1.55 kg.  Broiler chickens are raised primarily for meat rather than to lay eggs. These poultry are often white and are bred to be large and very healthy, often with more breast meat for the consumer market. Broiler chicken breeds grow very fast and offer good value in terms of protein and calories.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2349,22 +2365,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Fargo Safe Dry Fish (Chingri Shutki)</t>
+          <t>Fargo Safe Dry Fish (Churi Shutki)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>250 gm</t>
+          <t>100 gm</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>৳ 290</t>
+          <t>৳ 305</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Fargo is introducing safe and Organic Chingri Dry Fish (from World Bank, IFAD &amp; PKSF supported Safe Dry Fish Project). This quality protein and nutrient rich sea dry fish has iodine*, high-quality protein, OMEGA-3 Fatty Acid, Zinc, Calcium, copper and selenium. It is 100% natural and hygienically processed with no added preservatives.</t>
+          <t>Fargo is introducing safe and Organic Churi Dry Fish (from World Bank, IFAD &amp; PKSF supported Safe Dry Fish Project). This quality protein and nutrient rich sea dry fish has iodine*, high-quality protein, OMEGA-3 Fatty Acid, Zinc, Calcium, copper and selenium. It is 100% natural and hygienically processed with no added preservatives.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2376,22 +2392,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Fargo Safe Dry Fish (Churi Shutki)</t>
+          <t>Kazi Farms Kitchen Kechki Dried Fish</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>100 gm</t>
+          <t>125 gm</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>৳ 305</t>
+          <t>৳ 280</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Fargo is introducing safe and Organic Churi Dry Fish (from World Bank, IFAD &amp; PKSF supported Safe Dry Fish Project). This quality protein and nutrient rich sea dry fish has iodine*, high-quality protein, OMEGA-3 Fatty Acid, Zinc, Calcium, copper and selenium. It is 100% natural and hygienically processed with no added preservatives.</t>
+          <t>Kazi Farms Kitchen Kechki Dried Fish is a high-quality and nutritious food product made from fresh and clean Kechki fish that are caught from freshwater sources. The fish are carefully cleaned, salted, and dried using traditional methods to preserve their taste and nutritional value</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2607,24 +2623,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Radhuni Biryani Masala</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>40 gm</t>
-        </is>
-      </c>
+          <t>Fresh Haleem Mix 200 gm And Halim Meat (Beef) ± 20 gm 300 gm (Combo Offer)</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>৳ 60</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Specially made mixed spices for mutton, beef, and chicken biryani. The mixing of different spices maintains the standard recipe to prepare delicious Biryani.</t>
-        </is>
-      </c>
+          <t>৳ 259</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>Ready Mix</t>
@@ -2661,20 +2669,24 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Dekko Shahi Shemai</t>
+          <t>Radhuni Shemai</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>180 gm</t>
+          <t>200 gm</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>৳ 40</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>৳ 45</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Radhuni shemai has superb taste. it is smooth, lean &amp; thin and easy to prepare. Radhuni shemai is hygienically manufactured from finest quality flour which ensures delicious jorda shemai, milk shemai &amp; falooda.</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
           <t>Shemai &amp; Suji</t>
@@ -2684,24 +2696,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Cock Vermicelli (Shemai)</t>
+          <t>Dekko Shahi Shemai</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>200 gm</t>
+          <t>180 gm</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>৳ 45</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Cock Vermicelli (Shemai) made of pure flour. Its very tasty and healthy. Cock Vermically (Shemai) can be the nice dessert for your family.  Manufactured by: Hashem Foods Ltd.</t>
-        </is>
-      </c>
+          <t>৳ 40</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
           <t>Shemai &amp; Suji</t>
@@ -2762,17 +2770,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2 ltr</t>
+          <t>5 ltr</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>৳ 328</t>
+          <t>৳ 800</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">21 years of heritage.  First Vitamin A fortified Soyabean Oil.  Increases immunity.  Strengthens bone &amp; teeth. </t>
+          <t>First Vitamin A fortified Soyabean Oil.  Increases immunity.  Strengthens bone &amp; teeth.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2784,22 +2792,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fresh Fortified Soyabean Oil</t>
+          <t>Rupchanda Fortified Soyabean Oil</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5 ltr</t>
+          <t>2 ltr</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>৳ 800</t>
+          <t>৳ 328</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Fresh Fortified Soyabean Oil follows 3 steps of refining process-Perfect Degumming &amp; Neutralization, Balanced De-colorization and Five steps Deodorization to ensure right ratio of Omega 3 &amp; 6 and intact Beta-carotene in Soyabean Oil. Fresh soyabean oil contain vitamin A. Its fresh and healthy.</t>
+          <t xml:space="preserve">21 years of heritage.  First Vitamin A fortified Soyabean Oil.  Increases immunity.  Strengthens bone &amp; teeth. </t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2938,22 +2946,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fit Food Chia Seed</t>
+          <t>Ligion Black Seed With Sesame Seed</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>200 gm</t>
+          <t>100 gm</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>৳ 320</t>
+          <t>৳ 130</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Best Grade Chia Seed (Good Source of Fibre, Minerals and Omega Fatty Acid )  Benefits of Chia Seeds:  1. The High Fiber and Protein Content in Chia Seeds May Help You Lose Weight 2. Chia Seeds Are Loaded With Antioxidants 3. Almost All the Carbs in Them Are Fiber 4. Chia Seeds Are High in Quality Protein 5. Chia Seeds Deliver a Massive Amount of Nutrients With Very Few Calories 6. Chia Seeds Are High in Omega-3 Fatty Acids 7. Chia Seeds May Lower Your Risk of Heart Disease Given that chia seeds are high in fiber, protein an 8. They’re High in Many Important Bone Nutrients 9. Chia Seeds May Reduce Blood Sugar Levels 10. They May Reduce Chronic Inflammation 11. Chia Seeds Are Easy to Incorporate Into Your Diet</t>
+          <t xml:space="preserve">১। মায়ের স্তনে দুধ বৃদ্ধি, ২। ডায়াবেটিস কমায়, ৩। হাই ব্লাডপ্রেসার নিয়ন্ত্রণ করে, ৪। স্মরণশক্তি বৃদ্ধি করে, ৫। সর্দি, কাশি, এ্যাজমা দূর করে, ৬। পুরুষত্বহীনতা দূর করে, ৭। হার্টের রোগ দূর করে, ৮। মাথার উকুন ও খুশকি দূর করে, ৯। চুল পড়া ও চুল পাকা রোধ করে, ১০। মাথা ধরা দূর করে, ১১। ব্যাথা ও বাত রোগ দূর করে, ১২। পিঠ ও কোমরে ব্যাথা কমায়, ১৩। ক্ষত ও চর্মরোগ দূর করে, ১৪। সর্দি, কাশি, এ্যাজমা, কফ ও গলা ব্যথায় প্রতিদিন ২ বার আধা চামচ করে কালোজিরার তৈল মধুসহ সেবন করুন। সকালে ও রাতে শোয়ার পূর্বে বুকে ও পিঠে কালোজিরার তৈল মালিশ করুন। </t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3204,22 +3212,22 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Chicken Eggs (Special Offer)</t>
+          <t>Duck Eggs (Hasher Dim)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>12 pcs</t>
+          <t>6 pcs</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>৳ 109</t>
+          <t>৳ 99</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Eggs are an all-natural source of high-quality protein and a number of other nutrients, all for 70 calories an egg. 100% fresh and healthy.</t>
+          <t xml:space="preserve">Egg Weight (Per Pc): 70-80 gm   Locally Sourced; Duck Eggs are an all-natural source of high-quality protein and a number of other nutrients. Duck egg is a good source of Protein, Riboflavin, Folate, Iron and Phosphorus, and a very good source of Vitamin B12 and Selenium. Eggs are an all-natural source of high-quality protein and a number of other nutrients, all for 70 calories an egg. Cost-effective and versatile, the unique nutritional composition of eggs can help meet a variety of nutrient needs of children through older adults. It also good for weight management, muscle strength, healthy pregnancy, brain function, eye health and more. 100% fresh and healthy. </t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3578,22 +3586,22 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Chicken Eggs (Special Offer)</t>
+          <t>Duck Eggs (Hasher Dim)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>12 pcs</t>
+          <t>6 pcs</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>৳ 109</t>
+          <t>৳ 99</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Eggs are an all-natural source of high-quality protein and a number of other nutrients, all for 70 calories an egg. 100% fresh and healthy.</t>
+          <t xml:space="preserve">Egg Weight (Per Pc): 70-80 gm   Locally Sourced; Duck Eggs are an all-natural source of high-quality protein and a number of other nutrients. Duck egg is a good source of Protein, Riboflavin, Folate, Iron and Phosphorus, and a very good source of Vitamin B12 and Selenium. Eggs are an all-natural source of high-quality protein and a number of other nutrients, all for 70 calories an egg. Cost-effective and versatile, the unique nutritional composition of eggs can help meet a variety of nutrient needs of children through older adults. It also good for weight management, muscle strength, healthy pregnancy, brain function, eye health and more. 100% fresh and healthy. </t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3605,12 +3613,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Ispahani Mirzapore Tea Bag</t>
+          <t>Fresh Premium Black Tea</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>50 pcs</t>
+          <t>200 gm</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3620,7 +3628,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tea leaves are a natural source of goodness. Ispahani Mirzapore Tea is very special blent made from tea leaves of the garden of a Bangladesh. Ispahani Mirzapore Tea Bag is a blend of cheer and refresher. </t>
+          <t>Fresh Premium Black Tea is a type of tea made from the leaves of the Camellia sinensis plant that have undergone a complete oxidation process, resulting in a robust and flavorful brew. Black tea is known for its strong flavor, dark color, and caffeine content, making it a popular choice for tea enthusiasts.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3632,24 +3640,20 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Brooke Bond Taaza Black Tea</t>
+          <t>Revival Karak Masala Tea</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>150 gm</t>
+          <t>200 gm</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>৳ 100</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>In order to stay on top of your packed day, all you need is a clear mind – what's better than a cup of new Brooke Bond Taaza to refresh &amp; clear your mind. Because only new Brooke Bond Taaza is a tea with High Quality fresh Tea Leaves, packed with the Natural Goodness of Theanine, that helps to clear your mind and enables you to manage the demands of everyday life. This tea is perfect for those Spirited Aspirers who believe that the brighter future of their family is the center of their universe. Our world-class tea tasters and experts blend the tea that results in the exceptional colour, superior taste and impeccable aroma of each “Dana” of our brand. Strong processes ensure that the quality remains consistent throughout the year. Taaza makes sure that this phenomenal journey also resonates in every end cup as absolute refreshment!</t>
-        </is>
-      </c>
+          <t>৳ 170</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
           <t>Tea &amp; Coffee</t>
@@ -3952,22 +3956,22 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Cadbury Dairy Milk Silk Oreo Chocolate</t>
+          <t>Amul Dark Chocolate</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>60 gm</t>
+          <t>40 gm</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>৳ 150</t>
+          <t>৳ 129</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Product Origin:India   Description:  • Cadbury Dairy Milk Silk is all about regaling in the richness and creaminess of the chocolate. Indulge in a rich, smooth and creamy celebration.  • Silk: The classic taste of Cadbury Dairy Milk chocolates only more creamy, more smooth, more indulging.  • Cadbury Dairy Milk Silk is made with a glass and a half of milk.  • This pack is perfect to indulge in all alone or as a gift for your special someone.  • Every bar is made from 100% sustainable cocoa.  • Suitable for vegetarians.</t>
+          <t xml:space="preserve">Origin: India Amul Dark Chocolate is made with the finest ingredients and delicious cocoa. For a better texture, the finest particle size (approx. 20 microns) is achieved through world-class refining, leaving you to indulge in the exquisite taste of rich dark chocolate. • 55% dark chocolate • No milk solids • No vegetable fat • Pure cocoa butter &amp; solids </t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4214,24 +4218,20 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Panda Authentic Chinese Noodles</t>
+          <t>Mr.Noodles Magic Masala Easy Instant</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>300 gm</t>
+          <t>496 gm</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>৳ 60</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Panda Authentic Chinese Noodles is a brand of noodles that offers a taste and texture reminiscent of traditional Chinese cuisine. These noodles are commonly used in a variety of Chinese dishes, such as stir-fries, soups, and noodle-based recipes.</t>
-        </is>
-      </c>
+          <t>৳ 160</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
           <t>Noodles</t>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>185 gm</t>
+          <t>250 gm</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -5303,17 +5303,17 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Stainless Steel Spatula</t>
+          <t>Cake Mold</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>each</t>
+          <t>3 pcs</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>৳ 239</t>
+          <t>৳ 135</t>
         </is>
       </c>
       <c r="D138" t="inlineStr"/>
@@ -5326,22 +5326,22 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Transparent Disposable Piping Bags (8.5"x12.5")</t>
+          <t>Small Measurement Mug</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>100 pcs</t>
+          <t>each</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>৳ 469</t>
+          <t>৳ 179</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Piping bags are necessary for cake decoration. Fill these piping bags with cream and squeeze these with your hand to make designs on the cake. You can fit nozzles to these piping bags for designing easily.</t>
+          <t xml:space="preserve">500 ml, Material: Heavy plastic, Made in china </t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -5407,22 +5407,22 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>AG Food Chicken Salami 11-12 pcs</t>
+          <t>Kazi Farms Kitchen Chicken Spicy Meat Ball</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>200 gm</t>
+          <t>250 gm</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>৳ 250</t>
+          <t>৳ 195</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Country Of Origin: Bangladesh</t>
+          <t>Kazi Farms Kitchen chicken meatballs combine the incredible sort of Italian Style with a rich ingredient. Mixed with chicken and some rich flavor.They can be served as an appetizer, added to pasta dishes, used in sandwiches, or eaten as a snack.</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -5434,22 +5434,22 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>AG Food Chicken Mini Samosa</t>
+          <t>AG Food Chicken Salami 11-12 pcs</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>250 gm</t>
+          <t>200 gm</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>৳ 220</t>
+          <t>৳ 250</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>23-25 pcs crispy and delicious Chicken Mini Samosa.Storage:Keep frozen (-18°C or below). Do not refreeze once defrosted.Filling: Chicken meat, Salt, Sugar, Spices, Green Chili, Onion, and Soybean Oil.Pastry: Flour, Corn Starch, Salt, Water &amp; Soybean Oil.</t>
+          <t>Country Of Origin: Bangladesh</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">

</xml_diff>